<commit_message>
Our data runs better now
</commit_message>
<xml_diff>
--- a/Data/OurData.xlsx
+++ b/Data/OurData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA9D9ED-6EE0-DE4A-9C5A-40AA9A0123A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C7FC64-55A7-024F-AF74-D8B1CC921F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" activeTab="2" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" activeTab="4" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualisation" sheetId="7" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Arcs" sheetId="1" r:id="rId10"/>
     <sheet name="Traders" sheetId="3" r:id="rId11"/>
     <sheet name="Commodities" sheetId="4" r:id="rId12"/>
+    <sheet name="Probabilities" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="277">
   <si>
     <t>ID</t>
   </si>
@@ -866,6 +867,18 @@
   <si>
     <t>Temp</t>
   </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Total Hours</t>
+  </si>
+  <si>
+    <t>Dummy pipe 1</t>
+  </si>
+  <si>
+    <t>Dummy pipe 2</t>
+  </si>
 </sst>
 </file>
 
@@ -1032,7 +1045,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1127,6 +1140,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1134,7 +1158,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -1186,6 +1210,11 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1210,7 +1239,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1219,13 +1248,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1608,10 +1632,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902688A-D2A3-854F-B341-C0BEC53AF991}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1750,7 +1774,7 @@
         <v>5</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J50" si="0">IF(I3=100,"Capacity unknown","")</f>
+        <f t="shared" ref="J3:J52" si="0">IF(I3=100,"Capacity unknown","")</f>
         <v/>
       </c>
       <c r="K3" s="1">
@@ -3944,6 +3968,60 @@
         <v>1</v>
       </c>
       <c r="N50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="32">
+        <v>50</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="I51" s="35">
+        <v>100</v>
+      </c>
+      <c r="J51" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>Capacity unknown</v>
+      </c>
+      <c r="M51" s="2">
+        <v>1</v>
+      </c>
+      <c r="N51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="32">
+        <v>51</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I52" s="35">
+        <v>100</v>
+      </c>
+      <c r="J52" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>Capacity unknown</v>
+      </c>
+      <c r="M52" s="2">
+        <v>1</v>
+      </c>
+      <c r="N52" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4421,6 +4499,80 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FD9D31-8EFB-9D43-A52A-8F2DB4E9DCA7}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>C2/SUM($C$2:$C$5)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B5" si="0">C3/SUM($C$2:$C$5)</f>
+        <v>0.125</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCC4DE0-7BAC-1F4D-92A3-44AE62829735}">
   <dimension ref="A1:C10"/>
@@ -4547,7 +4699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3F5746-A1B1-6F4F-9762-CACD4A91B5F2}">
   <dimension ref="A1:AI67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -4590,39 +4742,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="32" t="s">
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -9311,14 +9463,14 @@
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="44">
+      <c r="C47" s="1"/>
+      <c r="D47" s="31">
         <v>3.23</v>
       </c>
-      <c r="E47" s="44">
+      <c r="E47" s="31">
         <v>56.55</v>
       </c>
       <c r="F47" s="1"/>
@@ -9415,14 +9567,14 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="45">
+      <c r="C48" s="1"/>
+      <c r="D48" s="23">
         <v>3.330503000000022</v>
       </c>
-      <c r="E48" s="45">
+      <c r="E48" s="23">
         <v>56.490369000000037</v>
       </c>
       <c r="F48" s="1"/>
@@ -11196,10 +11348,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8235E03E-FBB7-334A-A23D-60160D8DDD28}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="A4" sqref="A4:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11208,195 +11360,235 @@
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33">
-        <v>1</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
+      <c r="B1" s="38">
+        <v>1</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="33">
-        <v>1</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
+      <c r="B2" s="38">
+        <v>1</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="36"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="str">
+      <c r="B4" s="5" t="str">
         <f>'Demand Stage 2'!B4</f>
         <v>ST.FERGUS</v>
       </c>
-      <c r="C5" s="5" t="str">
+      <c r="C4" s="5" t="str">
         <f>'Demand Stage 2'!C4</f>
         <v>EASINGTON</v>
       </c>
-      <c r="D5" s="5" t="str">
+      <c r="D4" s="5" t="str">
         <f>'Demand Stage 2'!D4</f>
         <v>TEESSIDE</v>
       </c>
-      <c r="E5" s="5" t="str">
+      <c r="E4" s="5" t="str">
         <f>'Demand Stage 2'!E4</f>
         <v>EMDEN</v>
       </c>
-      <c r="F5" s="5" t="str">
+      <c r="F4" s="5" t="str">
         <f>'Demand Stage 2'!F4</f>
         <v>EMDEN 2</v>
       </c>
-      <c r="G5" s="5" t="str">
+      <c r="G4" s="5" t="str">
         <f>'Demand Stage 2'!G4</f>
         <v>ZEEBRUGGE</v>
       </c>
-      <c r="H5" s="5" t="str">
+      <c r="H4" s="5" t="str">
         <f>'Demand Stage 2'!H4</f>
         <v>DUNKERQUE</v>
       </c>
-      <c r="I5" s="5" t="str">
+      <c r="I4" s="5" t="str">
         <f>'Demand Stage 2'!I4</f>
         <v>POLAND</v>
       </c>
-      <c r="J5" s="6" t="str">
+      <c r="J4" s="6" t="str">
         <f>'Demand Stage 2'!J4</f>
         <v>ST.FERGUS</v>
       </c>
-      <c r="K5" s="6" t="str">
+      <c r="K4" s="6" t="str">
         <f>'Demand Stage 2'!K4</f>
         <v>EASINGTON</v>
       </c>
-      <c r="L5" s="6" t="str">
+      <c r="L4" s="6" t="str">
         <f>'Demand Stage 2'!L4</f>
         <v>TEESSIDE</v>
       </c>
-      <c r="M5" s="6" t="str">
+      <c r="M4" s="6" t="str">
         <f>'Demand Stage 2'!M4</f>
         <v>EMDEN</v>
       </c>
-      <c r="N5" s="6" t="str">
+      <c r="N4" s="6" t="str">
         <f>'Demand Stage 2'!N4</f>
         <v>EMDEN 2</v>
       </c>
-      <c r="O5" s="6" t="str">
+      <c r="O4" s="6" t="str">
         <f>'Demand Stage 2'!O4</f>
         <v>ZEEBRUGGE</v>
       </c>
-      <c r="P5" s="6" t="str">
+      <c r="P4" s="6" t="str">
         <f>'Demand Stage 2'!P4</f>
         <v>DUNKERQUE</v>
       </c>
-      <c r="Q5" s="6" t="str">
+      <c r="Q4" s="6" t="str">
         <f>'Demand Stage 2'!Q4</f>
         <v>POLAND</v>
       </c>
     </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <f>'Demand Stage 2'!B43</f>
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <f>'Demand Stage 2'!C43</f>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2">
+        <f>'Demand Stage 2'!D43</f>
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <f>'Demand Stage 2'!E43</f>
+        <v>40</v>
+      </c>
+      <c r="F5" s="2">
+        <f>'Demand Stage 2'!F43</f>
+        <v>40</v>
+      </c>
+      <c r="G5" s="2">
+        <f>'Demand Stage 2'!G43</f>
+        <v>40</v>
+      </c>
+      <c r="H5" s="2">
+        <f>'Demand Stage 2'!H43</f>
+        <v>40</v>
+      </c>
+      <c r="I5" s="2">
+        <f>'Demand Stage 2'!I43</f>
+        <v>20</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+    </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2">
-        <f>'Demand Stage 2'!B43</f>
+        <f>'Demand Stage 2'!B44</f>
         <v>10</v>
       </c>
       <c r="C6" s="2">
-        <f>'Demand Stage 2'!C43</f>
+        <f>'Demand Stage 2'!C44</f>
         <v>10</v>
       </c>
       <c r="D6" s="2">
-        <f>'Demand Stage 2'!D43</f>
+        <f>'Demand Stage 2'!D44</f>
         <v>10</v>
       </c>
       <c r="E6" s="2">
-        <f>'Demand Stage 2'!E43</f>
+        <f>'Demand Stage 2'!E44</f>
+        <v>45</v>
+      </c>
+      <c r="F6" s="2">
+        <f>'Demand Stage 2'!F44</f>
+        <v>45</v>
+      </c>
+      <c r="G6" s="2">
+        <f>'Demand Stage 2'!G44</f>
         <v>40</v>
       </c>
-      <c r="F6" s="2">
-        <f>'Demand Stage 2'!F43</f>
-        <v>40</v>
-      </c>
-      <c r="G6" s="2">
-        <f>'Demand Stage 2'!G43</f>
-        <v>40</v>
-      </c>
       <c r="H6" s="2">
-        <f>'Demand Stage 2'!H43</f>
-        <v>40</v>
+        <f>'Demand Stage 2'!H44</f>
+        <v>45</v>
       </c>
       <c r="I6" s="2">
-        <f>'Demand Stage 2'!I43</f>
+        <f>'Demand Stage 2'!I44</f>
         <v>20</v>
       </c>
       <c r="J6" s="3">
@@ -11426,38 +11618,38 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
-        <f>'Demand Stage 2'!B44</f>
+        <f>'Demand Stage 2'!B45</f>
         <v>10</v>
       </c>
       <c r="C7" s="2">
-        <f>'Demand Stage 2'!C44</f>
+        <f>'Demand Stage 2'!C45</f>
         <v>10</v>
       </c>
       <c r="D7" s="2">
-        <f>'Demand Stage 2'!D44</f>
+        <f>'Demand Stage 2'!D45</f>
         <v>10</v>
       </c>
       <c r="E7" s="2">
-        <f>'Demand Stage 2'!E44</f>
-        <v>45</v>
+        <f>'Demand Stage 2'!E45</f>
+        <v>40</v>
       </c>
       <c r="F7" s="2">
-        <f>'Demand Stage 2'!F44</f>
-        <v>45</v>
+        <f>'Demand Stage 2'!F45</f>
+        <v>40</v>
       </c>
       <c r="G7" s="2">
-        <f>'Demand Stage 2'!G44</f>
+        <f>'Demand Stage 2'!G45</f>
         <v>40</v>
       </c>
       <c r="H7" s="2">
-        <f>'Demand Stage 2'!H44</f>
-        <v>45</v>
+        <f>'Demand Stage 2'!H45</f>
+        <v>35</v>
       </c>
       <c r="I7" s="2">
-        <f>'Demand Stage 2'!I44</f>
+        <f>'Demand Stage 2'!I45</f>
         <v>20</v>
       </c>
       <c r="J7" s="3">
@@ -11487,38 +11679,38 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
-        <f>'Demand Stage 2'!B45</f>
+        <f>'Demand Stage 2'!B46</f>
         <v>10</v>
       </c>
       <c r="C8" s="2">
-        <f>'Demand Stage 2'!C45</f>
+        <f>'Demand Stage 2'!C46</f>
         <v>10</v>
       </c>
       <c r="D8" s="2">
-        <f>'Demand Stage 2'!D45</f>
+        <f>'Demand Stage 2'!D46</f>
         <v>10</v>
       </c>
       <c r="E8" s="2">
-        <f>'Demand Stage 2'!E45</f>
+        <f>'Demand Stage 2'!E46</f>
+        <v>45</v>
+      </c>
+      <c r="F8" s="2">
+        <f>'Demand Stage 2'!F46</f>
+        <v>45</v>
+      </c>
+      <c r="G8" s="2">
+        <f>'Demand Stage 2'!G46</f>
         <v>40</v>
       </c>
-      <c r="F8" s="2">
-        <f>'Demand Stage 2'!F45</f>
+      <c r="H8" s="2">
+        <f>'Demand Stage 2'!H46</f>
         <v>40</v>
       </c>
-      <c r="G8" s="2">
-        <f>'Demand Stage 2'!G45</f>
-        <v>40</v>
-      </c>
-      <c r="H8" s="2">
-        <f>'Demand Stage 2'!H45</f>
-        <v>35</v>
-      </c>
       <c r="I8" s="2">
-        <f>'Demand Stage 2'!I45</f>
+        <f>'Demand Stage 2'!I46</f>
         <v>20</v>
       </c>
       <c r="J8" s="3">
@@ -11548,68 +11740,28 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2">
-        <f>'Demand Stage 2'!B46</f>
-        <v>10</v>
-      </c>
-      <c r="C9" s="2">
-        <f>'Demand Stage 2'!C46</f>
-        <v>10</v>
-      </c>
-      <c r="D9" s="2">
-        <f>'Demand Stage 2'!D46</f>
-        <v>10</v>
-      </c>
-      <c r="E9" s="2">
-        <f>'Demand Stage 2'!E46</f>
-        <v>45</v>
-      </c>
-      <c r="F9" s="2">
-        <f>'Demand Stage 2'!F46</f>
-        <v>45</v>
-      </c>
-      <c r="G9" s="2">
-        <f>'Demand Stage 2'!G46</f>
-        <v>40</v>
-      </c>
-      <c r="H9" s="2">
-        <f>'Demand Stage 2'!H46</f>
-        <v>40</v>
-      </c>
-      <c r="I9" s="2">
-        <f>'Demand Stage 2'!I46</f>
-        <v>20</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -11630,7 +11782,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -11651,7 +11803,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -11672,7 +11824,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -11693,7 +11845,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -11714,7 +11866,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -11735,7 +11887,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -11756,7 +11908,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -11777,7 +11929,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -11798,7 +11950,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -11819,7 +11971,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -11840,7 +11992,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -11861,7 +12013,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -11882,7 +12034,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -11903,7 +12055,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -11924,7 +12076,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -11945,7 +12097,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -11966,7 +12118,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -11987,7 +12139,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -12006,34 +12158,12 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>23</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="B1:Q1"/>
     <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="J3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12043,8 +12173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19292E87-5CF7-794D-A1AA-7C1926221C7B}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:I4"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12072,244 +12202,244 @@
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33">
-        <v>2</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33">
+      <c r="B1" s="38">
+        <v>5</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38">
         <f>B1+Parameters!$B$5</f>
-        <v>6</v>
-      </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33">
+        <v>9</v>
+      </c>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38">
         <f>R1+Parameters!$B$5</f>
-        <v>10</v>
-      </c>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="33"/>
-      <c r="AU1" s="33"/>
-      <c r="AV1" s="33"/>
-      <c r="AW1" s="33"/>
-      <c r="AX1" s="33">
+        <v>13</v>
+      </c>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38"/>
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="38">
         <f>AH1+Parameters!$B$5</f>
-        <v>14</v>
-      </c>
-      <c r="AY1" s="33"/>
-      <c r="AZ1" s="33"/>
-      <c r="BA1" s="33"/>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="33"/>
-      <c r="BE1" s="33"/>
-      <c r="BF1" s="33"/>
-      <c r="BG1" s="33"/>
-      <c r="BH1" s="33"/>
-      <c r="BI1" s="33"/>
-      <c r="BJ1" s="33"/>
-      <c r="BK1" s="33"/>
-      <c r="BL1" s="33"/>
-      <c r="BM1" s="33"/>
+        <v>17</v>
+      </c>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38"/>
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38"/>
+      <c r="BD1" s="38"/>
+      <c r="BE1" s="38"/>
+      <c r="BF1" s="38"/>
+      <c r="BG1" s="38"/>
+      <c r="BH1" s="38"/>
+      <c r="BI1" s="38"/>
+      <c r="BJ1" s="38"/>
+      <c r="BK1" s="38"/>
+      <c r="BL1" s="38"/>
+      <c r="BM1" s="38"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="38">
         <v>0.25</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38">
         <f>B2</f>
         <v>0.25</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33">
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38">
         <f>B2</f>
         <v>0.25</v>
       </c>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33">
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="38">
         <f>B2</f>
         <v>0.25</v>
       </c>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="33"/>
-      <c r="BH2" s="33"/>
-      <c r="BI2" s="33"/>
-      <c r="BJ2" s="33"/>
-      <c r="BK2" s="33"/>
-      <c r="BL2" s="33"/>
-      <c r="BM2" s="33"/>
+      <c r="AY2" s="38"/>
+      <c r="AZ2" s="38"/>
+      <c r="BA2" s="38"/>
+      <c r="BB2" s="38"/>
+      <c r="BC2" s="38"/>
+      <c r="BD2" s="38"/>
+      <c r="BE2" s="38"/>
+      <c r="BF2" s="38"/>
+      <c r="BG2" s="38"/>
+      <c r="BH2" s="38"/>
+      <c r="BI2" s="38"/>
+      <c r="BJ2" s="38"/>
+      <c r="BK2" s="38"/>
+      <c r="BL2" s="38"/>
+      <c r="BM2" s="38"/>
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="37" t="s">
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="38" t="s">
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="42"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="38"/>
-      <c r="AD3" s="38"/>
-      <c r="AE3" s="38"/>
-      <c r="AF3" s="38"/>
-      <c r="AG3" s="38"/>
-      <c r="AH3" s="37" t="s">
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="43"/>
+      <c r="AH3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37"/>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="37"/>
-      <c r="AO3" s="37"/>
-      <c r="AP3" s="38" t="s">
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
+      <c r="AM3" s="42"/>
+      <c r="AN3" s="42"/>
+      <c r="AO3" s="42"/>
+      <c r="AP3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="38"/>
-      <c r="AR3" s="38"/>
-      <c r="AS3" s="38"/>
-      <c r="AT3" s="38"/>
-      <c r="AU3" s="38"/>
-      <c r="AV3" s="38"/>
-      <c r="AW3" s="38"/>
-      <c r="AX3" s="37" t="s">
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="43"/>
+      <c r="AS3" s="43"/>
+      <c r="AT3" s="43"/>
+      <c r="AU3" s="43"/>
+      <c r="AV3" s="43"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AY3" s="37"/>
-      <c r="AZ3" s="37"/>
-      <c r="BA3" s="37"/>
-      <c r="BB3" s="37"/>
-      <c r="BC3" s="37"/>
-      <c r="BD3" s="37"/>
-      <c r="BE3" s="37"/>
-      <c r="BF3" s="38" t="s">
+      <c r="AY3" s="42"/>
+      <c r="AZ3" s="42"/>
+      <c r="BA3" s="42"/>
+      <c r="BB3" s="42"/>
+      <c r="BC3" s="42"/>
+      <c r="BD3" s="42"/>
+      <c r="BE3" s="42"/>
+      <c r="BF3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="BG3" s="38"/>
-      <c r="BH3" s="38"/>
-      <c r="BI3" s="38"/>
-      <c r="BJ3" s="38"/>
-      <c r="BK3" s="38"/>
-      <c r="BL3" s="38"/>
-      <c r="BM3" s="38"/>
+      <c r="BG3" s="43"/>
+      <c r="BH3" s="43"/>
+      <c r="BI3" s="43"/>
+      <c r="BJ3" s="43"/>
+      <c r="BK3" s="43"/>
+      <c r="BL3" s="43"/>
+      <c r="BM3" s="43"/>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -15482,6 +15612,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AH1:AW1"/>
+    <mergeCell ref="AH2:AW2"/>
+    <mergeCell ref="AH3:AO3"/>
+    <mergeCell ref="AP3:AW3"/>
+    <mergeCell ref="AX1:BM1"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="AX3:BE3"/>
+    <mergeCell ref="BF3:BM3"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="B1:Q1"/>
@@ -15490,14 +15628,6 @@
     <mergeCell ref="R2:AG2"/>
     <mergeCell ref="R3:Y3"/>
     <mergeCell ref="Z3:AG3"/>
-    <mergeCell ref="AH1:AW1"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="AH3:AO3"/>
-    <mergeCell ref="AP3:AW3"/>
-    <mergeCell ref="AX1:BM1"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="AX3:BE3"/>
-    <mergeCell ref="BF3:BM3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15507,8 +15637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7506CF-850A-ED42-956F-025E5A994524}">
   <dimension ref="A1:IW33"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="IH1" sqref="IH1:IW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15522,1234 +15652,1234 @@
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33">
-        <v>18</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33">
+      <c r="B1" s="38">
+        <v>21</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38">
         <f>B1+Parameters!$B$5</f>
-        <v>22</v>
-      </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33">
+        <v>25</v>
+      </c>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38">
         <f>R1+Parameters!$B$5</f>
-        <v>26</v>
-      </c>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="33"/>
-      <c r="AU1" s="33"/>
-      <c r="AV1" s="33"/>
-      <c r="AW1" s="33"/>
-      <c r="AX1" s="33">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38"/>
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="38">
         <f>AH1+Parameters!$B$5</f>
-        <v>30</v>
-      </c>
-      <c r="AY1" s="33"/>
-      <c r="AZ1" s="33"/>
-      <c r="BA1" s="33"/>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="33"/>
-      <c r="BE1" s="33"/>
-      <c r="BF1" s="33"/>
-      <c r="BG1" s="33"/>
-      <c r="BH1" s="33"/>
-      <c r="BI1" s="33"/>
-      <c r="BJ1" s="33"/>
-      <c r="BK1" s="33"/>
-      <c r="BL1" s="33"/>
-      <c r="BM1" s="33"/>
-      <c r="BN1" s="33">
+        <v>33</v>
+      </c>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38"/>
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38"/>
+      <c r="BD1" s="38"/>
+      <c r="BE1" s="38"/>
+      <c r="BF1" s="38"/>
+      <c r="BG1" s="38"/>
+      <c r="BH1" s="38"/>
+      <c r="BI1" s="38"/>
+      <c r="BJ1" s="38"/>
+      <c r="BK1" s="38"/>
+      <c r="BL1" s="38"/>
+      <c r="BM1" s="38"/>
+      <c r="BN1" s="38">
         <f>AX1+Parameters!$B$5</f>
-        <v>34</v>
-      </c>
-      <c r="BO1" s="33"/>
-      <c r="BP1" s="33"/>
-      <c r="BQ1" s="33"/>
-      <c r="BR1" s="33"/>
-      <c r="BS1" s="33"/>
-      <c r="BT1" s="33"/>
-      <c r="BU1" s="33"/>
-      <c r="BV1" s="33"/>
-      <c r="BW1" s="33"/>
-      <c r="BX1" s="33"/>
-      <c r="BY1" s="33"/>
-      <c r="BZ1" s="33"/>
-      <c r="CA1" s="33"/>
-      <c r="CB1" s="33"/>
-      <c r="CC1" s="33"/>
-      <c r="CD1" s="33">
+        <v>37</v>
+      </c>
+      <c r="BO1" s="38"/>
+      <c r="BP1" s="38"/>
+      <c r="BQ1" s="38"/>
+      <c r="BR1" s="38"/>
+      <c r="BS1" s="38"/>
+      <c r="BT1" s="38"/>
+      <c r="BU1" s="38"/>
+      <c r="BV1" s="38"/>
+      <c r="BW1" s="38"/>
+      <c r="BX1" s="38"/>
+      <c r="BY1" s="38"/>
+      <c r="BZ1" s="38"/>
+      <c r="CA1" s="38"/>
+      <c r="CB1" s="38"/>
+      <c r="CC1" s="38"/>
+      <c r="CD1" s="38">
         <f>BN1+Parameters!$B$5</f>
-        <v>38</v>
-      </c>
-      <c r="CE1" s="33"/>
-      <c r="CF1" s="33"/>
-      <c r="CG1" s="33"/>
-      <c r="CH1" s="33"/>
-      <c r="CI1" s="33"/>
-      <c r="CJ1" s="33"/>
-      <c r="CK1" s="33"/>
-      <c r="CL1" s="33"/>
-      <c r="CM1" s="33"/>
-      <c r="CN1" s="33"/>
-      <c r="CO1" s="33"/>
-      <c r="CP1" s="33"/>
-      <c r="CQ1" s="33"/>
-      <c r="CR1" s="33"/>
-      <c r="CS1" s="33"/>
-      <c r="CT1" s="33">
+        <v>41</v>
+      </c>
+      <c r="CE1" s="38"/>
+      <c r="CF1" s="38"/>
+      <c r="CG1" s="38"/>
+      <c r="CH1" s="38"/>
+      <c r="CI1" s="38"/>
+      <c r="CJ1" s="38"/>
+      <c r="CK1" s="38"/>
+      <c r="CL1" s="38"/>
+      <c r="CM1" s="38"/>
+      <c r="CN1" s="38"/>
+      <c r="CO1" s="38"/>
+      <c r="CP1" s="38"/>
+      <c r="CQ1" s="38"/>
+      <c r="CR1" s="38"/>
+      <c r="CS1" s="38"/>
+      <c r="CT1" s="38">
         <f>CD1+Parameters!$B$5</f>
-        <v>42</v>
-      </c>
-      <c r="CU1" s="33"/>
-      <c r="CV1" s="33"/>
-      <c r="CW1" s="33"/>
-      <c r="CX1" s="33"/>
-      <c r="CY1" s="33"/>
-      <c r="CZ1" s="33"/>
-      <c r="DA1" s="33"/>
-      <c r="DB1" s="33"/>
-      <c r="DC1" s="33"/>
-      <c r="DD1" s="33"/>
-      <c r="DE1" s="33"/>
-      <c r="DF1" s="33"/>
-      <c r="DG1" s="33"/>
-      <c r="DH1" s="33"/>
-      <c r="DI1" s="33"/>
-      <c r="DJ1" s="33">
+        <v>45</v>
+      </c>
+      <c r="CU1" s="38"/>
+      <c r="CV1" s="38"/>
+      <c r="CW1" s="38"/>
+      <c r="CX1" s="38"/>
+      <c r="CY1" s="38"/>
+      <c r="CZ1" s="38"/>
+      <c r="DA1" s="38"/>
+      <c r="DB1" s="38"/>
+      <c r="DC1" s="38"/>
+      <c r="DD1" s="38"/>
+      <c r="DE1" s="38"/>
+      <c r="DF1" s="38"/>
+      <c r="DG1" s="38"/>
+      <c r="DH1" s="38"/>
+      <c r="DI1" s="38"/>
+      <c r="DJ1" s="38">
         <f>CT1+Parameters!$B$5</f>
-        <v>46</v>
-      </c>
-      <c r="DK1" s="33"/>
-      <c r="DL1" s="33"/>
-      <c r="DM1" s="33"/>
-      <c r="DN1" s="33"/>
-      <c r="DO1" s="33"/>
-      <c r="DP1" s="33"/>
-      <c r="DQ1" s="33"/>
-      <c r="DR1" s="33"/>
-      <c r="DS1" s="33"/>
-      <c r="DT1" s="33"/>
-      <c r="DU1" s="33"/>
-      <c r="DV1" s="33"/>
-      <c r="DW1" s="33"/>
-      <c r="DX1" s="33"/>
-      <c r="DY1" s="33"/>
-      <c r="DZ1" s="33">
+        <v>49</v>
+      </c>
+      <c r="DK1" s="38"/>
+      <c r="DL1" s="38"/>
+      <c r="DM1" s="38"/>
+      <c r="DN1" s="38"/>
+      <c r="DO1" s="38"/>
+      <c r="DP1" s="38"/>
+      <c r="DQ1" s="38"/>
+      <c r="DR1" s="38"/>
+      <c r="DS1" s="38"/>
+      <c r="DT1" s="38"/>
+      <c r="DU1" s="38"/>
+      <c r="DV1" s="38"/>
+      <c r="DW1" s="38"/>
+      <c r="DX1" s="38"/>
+      <c r="DY1" s="38"/>
+      <c r="DZ1" s="38">
         <f>DJ1+Parameters!$B$5</f>
-        <v>50</v>
-      </c>
-      <c r="EA1" s="33"/>
-      <c r="EB1" s="33"/>
-      <c r="EC1" s="33"/>
-      <c r="ED1" s="33"/>
-      <c r="EE1" s="33"/>
-      <c r="EF1" s="33"/>
-      <c r="EG1" s="33"/>
-      <c r="EH1" s="33"/>
-      <c r="EI1" s="33"/>
-      <c r="EJ1" s="33"/>
-      <c r="EK1" s="33"/>
-      <c r="EL1" s="33"/>
-      <c r="EM1" s="33"/>
-      <c r="EN1" s="33"/>
-      <c r="EO1" s="33"/>
-      <c r="EP1" s="33">
+        <v>53</v>
+      </c>
+      <c r="EA1" s="38"/>
+      <c r="EB1" s="38"/>
+      <c r="EC1" s="38"/>
+      <c r="ED1" s="38"/>
+      <c r="EE1" s="38"/>
+      <c r="EF1" s="38"/>
+      <c r="EG1" s="38"/>
+      <c r="EH1" s="38"/>
+      <c r="EI1" s="38"/>
+      <c r="EJ1" s="38"/>
+      <c r="EK1" s="38"/>
+      <c r="EL1" s="38"/>
+      <c r="EM1" s="38"/>
+      <c r="EN1" s="38"/>
+      <c r="EO1" s="38"/>
+      <c r="EP1" s="38">
         <f>DZ1+Parameters!$B$5</f>
-        <v>54</v>
-      </c>
-      <c r="EQ1" s="33"/>
-      <c r="ER1" s="33"/>
-      <c r="ES1" s="33"/>
-      <c r="ET1" s="33"/>
-      <c r="EU1" s="33"/>
-      <c r="EV1" s="33"/>
-      <c r="EW1" s="33"/>
-      <c r="EX1" s="33"/>
-      <c r="EY1" s="33"/>
-      <c r="EZ1" s="33"/>
-      <c r="FA1" s="33"/>
-      <c r="FB1" s="33"/>
-      <c r="FC1" s="33"/>
-      <c r="FD1" s="33"/>
-      <c r="FE1" s="33"/>
-      <c r="FF1" s="33">
+        <v>57</v>
+      </c>
+      <c r="EQ1" s="38"/>
+      <c r="ER1" s="38"/>
+      <c r="ES1" s="38"/>
+      <c r="ET1" s="38"/>
+      <c r="EU1" s="38"/>
+      <c r="EV1" s="38"/>
+      <c r="EW1" s="38"/>
+      <c r="EX1" s="38"/>
+      <c r="EY1" s="38"/>
+      <c r="EZ1" s="38"/>
+      <c r="FA1" s="38"/>
+      <c r="FB1" s="38"/>
+      <c r="FC1" s="38"/>
+      <c r="FD1" s="38"/>
+      <c r="FE1" s="38"/>
+      <c r="FF1" s="38">
         <f>EP1+Parameters!$B$5</f>
-        <v>58</v>
-      </c>
-      <c r="FG1" s="33"/>
-      <c r="FH1" s="33"/>
-      <c r="FI1" s="33"/>
-      <c r="FJ1" s="33"/>
-      <c r="FK1" s="33"/>
-      <c r="FL1" s="33"/>
-      <c r="FM1" s="33"/>
-      <c r="FN1" s="33"/>
-      <c r="FO1" s="33"/>
-      <c r="FP1" s="33"/>
-      <c r="FQ1" s="33"/>
-      <c r="FR1" s="33"/>
-      <c r="FS1" s="33"/>
-      <c r="FT1" s="33"/>
-      <c r="FU1" s="33"/>
-      <c r="FV1" s="33">
+        <v>61</v>
+      </c>
+      <c r="FG1" s="38"/>
+      <c r="FH1" s="38"/>
+      <c r="FI1" s="38"/>
+      <c r="FJ1" s="38"/>
+      <c r="FK1" s="38"/>
+      <c r="FL1" s="38"/>
+      <c r="FM1" s="38"/>
+      <c r="FN1" s="38"/>
+      <c r="FO1" s="38"/>
+      <c r="FP1" s="38"/>
+      <c r="FQ1" s="38"/>
+      <c r="FR1" s="38"/>
+      <c r="FS1" s="38"/>
+      <c r="FT1" s="38"/>
+      <c r="FU1" s="38"/>
+      <c r="FV1" s="38">
         <f>FF1+Parameters!$B$5</f>
-        <v>62</v>
-      </c>
-      <c r="FW1" s="33"/>
-      <c r="FX1" s="33"/>
-      <c r="FY1" s="33"/>
-      <c r="FZ1" s="33"/>
-      <c r="GA1" s="33"/>
-      <c r="GB1" s="33"/>
-      <c r="GC1" s="33"/>
-      <c r="GD1" s="33"/>
-      <c r="GE1" s="33"/>
-      <c r="GF1" s="33"/>
-      <c r="GG1" s="33"/>
-      <c r="GH1" s="33"/>
-      <c r="GI1" s="33"/>
-      <c r="GJ1" s="33"/>
-      <c r="GK1" s="33"/>
-      <c r="GL1" s="33">
+        <v>65</v>
+      </c>
+      <c r="FW1" s="38"/>
+      <c r="FX1" s="38"/>
+      <c r="FY1" s="38"/>
+      <c r="FZ1" s="38"/>
+      <c r="GA1" s="38"/>
+      <c r="GB1" s="38"/>
+      <c r="GC1" s="38"/>
+      <c r="GD1" s="38"/>
+      <c r="GE1" s="38"/>
+      <c r="GF1" s="38"/>
+      <c r="GG1" s="38"/>
+      <c r="GH1" s="38"/>
+      <c r="GI1" s="38"/>
+      <c r="GJ1" s="38"/>
+      <c r="GK1" s="38"/>
+      <c r="GL1" s="38">
         <f>FV1+Parameters!$B$5</f>
-        <v>66</v>
-      </c>
-      <c r="GM1" s="33"/>
-      <c r="GN1" s="33"/>
-      <c r="GO1" s="33"/>
-      <c r="GP1" s="33"/>
-      <c r="GQ1" s="33"/>
-      <c r="GR1" s="33"/>
-      <c r="GS1" s="33"/>
-      <c r="GT1" s="33"/>
-      <c r="GU1" s="33"/>
-      <c r="GV1" s="33"/>
-      <c r="GW1" s="33"/>
-      <c r="GX1" s="33"/>
-      <c r="GY1" s="33"/>
-      <c r="GZ1" s="33"/>
-      <c r="HA1" s="33"/>
-      <c r="HB1" s="33">
+        <v>69</v>
+      </c>
+      <c r="GM1" s="38"/>
+      <c r="GN1" s="38"/>
+      <c r="GO1" s="38"/>
+      <c r="GP1" s="38"/>
+      <c r="GQ1" s="38"/>
+      <c r="GR1" s="38"/>
+      <c r="GS1" s="38"/>
+      <c r="GT1" s="38"/>
+      <c r="GU1" s="38"/>
+      <c r="GV1" s="38"/>
+      <c r="GW1" s="38"/>
+      <c r="GX1" s="38"/>
+      <c r="GY1" s="38"/>
+      <c r="GZ1" s="38"/>
+      <c r="HA1" s="38"/>
+      <c r="HB1" s="38">
         <f>GL1+Parameters!$B$5</f>
-        <v>70</v>
-      </c>
-      <c r="HC1" s="33"/>
-      <c r="HD1" s="33"/>
-      <c r="HE1" s="33"/>
-      <c r="HF1" s="33"/>
-      <c r="HG1" s="33"/>
-      <c r="HH1" s="33"/>
-      <c r="HI1" s="33"/>
-      <c r="HJ1" s="33"/>
-      <c r="HK1" s="33"/>
-      <c r="HL1" s="33"/>
-      <c r="HM1" s="33"/>
-      <c r="HN1" s="33"/>
-      <c r="HO1" s="33"/>
-      <c r="HP1" s="33"/>
-      <c r="HQ1" s="33"/>
-      <c r="HR1" s="33">
+        <v>73</v>
+      </c>
+      <c r="HC1" s="38"/>
+      <c r="HD1" s="38"/>
+      <c r="HE1" s="38"/>
+      <c r="HF1" s="38"/>
+      <c r="HG1" s="38"/>
+      <c r="HH1" s="38"/>
+      <c r="HI1" s="38"/>
+      <c r="HJ1" s="38"/>
+      <c r="HK1" s="38"/>
+      <c r="HL1" s="38"/>
+      <c r="HM1" s="38"/>
+      <c r="HN1" s="38"/>
+      <c r="HO1" s="38"/>
+      <c r="HP1" s="38"/>
+      <c r="HQ1" s="38"/>
+      <c r="HR1" s="38">
         <f>HB1+Parameters!$B$5</f>
-        <v>74</v>
-      </c>
-      <c r="HS1" s="33"/>
-      <c r="HT1" s="33"/>
-      <c r="HU1" s="33"/>
-      <c r="HV1" s="33"/>
-      <c r="HW1" s="33"/>
-      <c r="HX1" s="33"/>
-      <c r="HY1" s="33"/>
-      <c r="HZ1" s="33"/>
-      <c r="IA1" s="33"/>
-      <c r="IB1" s="33"/>
-      <c r="IC1" s="33"/>
-      <c r="ID1" s="33"/>
-      <c r="IE1" s="33"/>
-      <c r="IF1" s="33"/>
-      <c r="IG1" s="33"/>
-      <c r="IH1" s="33">
+        <v>77</v>
+      </c>
+      <c r="HS1" s="38"/>
+      <c r="HT1" s="38"/>
+      <c r="HU1" s="38"/>
+      <c r="HV1" s="38"/>
+      <c r="HW1" s="38"/>
+      <c r="HX1" s="38"/>
+      <c r="HY1" s="38"/>
+      <c r="HZ1" s="38"/>
+      <c r="IA1" s="38"/>
+      <c r="IB1" s="38"/>
+      <c r="IC1" s="38"/>
+      <c r="ID1" s="38"/>
+      <c r="IE1" s="38"/>
+      <c r="IF1" s="38"/>
+      <c r="IG1" s="38"/>
+      <c r="IH1" s="38">
         <f>HR1+Parameters!$B$5</f>
-        <v>78</v>
-      </c>
-      <c r="II1" s="33"/>
-      <c r="IJ1" s="33"/>
-      <c r="IK1" s="33"/>
-      <c r="IL1" s="33"/>
-      <c r="IM1" s="33"/>
-      <c r="IN1" s="33"/>
-      <c r="IO1" s="33"/>
-      <c r="IP1" s="33"/>
-      <c r="IQ1" s="33"/>
-      <c r="IR1" s="33"/>
-      <c r="IS1" s="33"/>
-      <c r="IT1" s="33"/>
-      <c r="IU1" s="33"/>
-      <c r="IV1" s="33"/>
-      <c r="IW1" s="33"/>
+        <v>81</v>
+      </c>
+      <c r="II1" s="38"/>
+      <c r="IJ1" s="38"/>
+      <c r="IK1" s="38"/>
+      <c r="IL1" s="38"/>
+      <c r="IM1" s="38"/>
+      <c r="IN1" s="38"/>
+      <c r="IO1" s="38"/>
+      <c r="IP1" s="38"/>
+      <c r="IQ1" s="38"/>
+      <c r="IR1" s="38"/>
+      <c r="IS1" s="38"/>
+      <c r="IT1" s="38"/>
+      <c r="IU1" s="38"/>
+      <c r="IV1" s="38"/>
+      <c r="IW1" s="38"/>
     </row>
     <row r="2" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="38">
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38">
         <f>B2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33">
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38">
         <f t="shared" ref="AH2" si="0">R2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33">
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="38">
         <f t="shared" ref="AX2" si="1">AH2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="33"/>
-      <c r="BH2" s="33"/>
-      <c r="BI2" s="33"/>
-      <c r="BJ2" s="33"/>
-      <c r="BK2" s="33"/>
-      <c r="BL2" s="33"/>
-      <c r="BM2" s="33"/>
-      <c r="BN2" s="33">
+      <c r="AY2" s="38"/>
+      <c r="AZ2" s="38"/>
+      <c r="BA2" s="38"/>
+      <c r="BB2" s="38"/>
+      <c r="BC2" s="38"/>
+      <c r="BD2" s="38"/>
+      <c r="BE2" s="38"/>
+      <c r="BF2" s="38"/>
+      <c r="BG2" s="38"/>
+      <c r="BH2" s="38"/>
+      <c r="BI2" s="38"/>
+      <c r="BJ2" s="38"/>
+      <c r="BK2" s="38"/>
+      <c r="BL2" s="38"/>
+      <c r="BM2" s="38"/>
+      <c r="BN2" s="38">
         <f t="shared" ref="BN2" si="2">AX2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="BO2" s="33"/>
-      <c r="BP2" s="33"/>
-      <c r="BQ2" s="33"/>
-      <c r="BR2" s="33"/>
-      <c r="BS2" s="33"/>
-      <c r="BT2" s="33"/>
-      <c r="BU2" s="33"/>
-      <c r="BV2" s="33"/>
-      <c r="BW2" s="33"/>
-      <c r="BX2" s="33"/>
-      <c r="BY2" s="33"/>
-      <c r="BZ2" s="33"/>
-      <c r="CA2" s="33"/>
-      <c r="CB2" s="33"/>
-      <c r="CC2" s="33"/>
-      <c r="CD2" s="33">
+      <c r="BO2" s="38"/>
+      <c r="BP2" s="38"/>
+      <c r="BQ2" s="38"/>
+      <c r="BR2" s="38"/>
+      <c r="BS2" s="38"/>
+      <c r="BT2" s="38"/>
+      <c r="BU2" s="38"/>
+      <c r="BV2" s="38"/>
+      <c r="BW2" s="38"/>
+      <c r="BX2" s="38"/>
+      <c r="BY2" s="38"/>
+      <c r="BZ2" s="38"/>
+      <c r="CA2" s="38"/>
+      <c r="CB2" s="38"/>
+      <c r="CC2" s="38"/>
+      <c r="CD2" s="38">
         <f t="shared" ref="CD2" si="3">BN2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="CE2" s="33"/>
-      <c r="CF2" s="33"/>
-      <c r="CG2" s="33"/>
-      <c r="CH2" s="33"/>
-      <c r="CI2" s="33"/>
-      <c r="CJ2" s="33"/>
-      <c r="CK2" s="33"/>
-      <c r="CL2" s="33"/>
-      <c r="CM2" s="33"/>
-      <c r="CN2" s="33"/>
-      <c r="CO2" s="33"/>
-      <c r="CP2" s="33"/>
-      <c r="CQ2" s="33"/>
-      <c r="CR2" s="33"/>
-      <c r="CS2" s="33"/>
-      <c r="CT2" s="33">
+      <c r="CE2" s="38"/>
+      <c r="CF2" s="38"/>
+      <c r="CG2" s="38"/>
+      <c r="CH2" s="38"/>
+      <c r="CI2" s="38"/>
+      <c r="CJ2" s="38"/>
+      <c r="CK2" s="38"/>
+      <c r="CL2" s="38"/>
+      <c r="CM2" s="38"/>
+      <c r="CN2" s="38"/>
+      <c r="CO2" s="38"/>
+      <c r="CP2" s="38"/>
+      <c r="CQ2" s="38"/>
+      <c r="CR2" s="38"/>
+      <c r="CS2" s="38"/>
+      <c r="CT2" s="38">
         <f t="shared" ref="CT2" si="4">CD2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="CU2" s="33"/>
-      <c r="CV2" s="33"/>
-      <c r="CW2" s="33"/>
-      <c r="CX2" s="33"/>
-      <c r="CY2" s="33"/>
-      <c r="CZ2" s="33"/>
-      <c r="DA2" s="33"/>
-      <c r="DB2" s="33"/>
-      <c r="DC2" s="33"/>
-      <c r="DD2" s="33"/>
-      <c r="DE2" s="33"/>
-      <c r="DF2" s="33"/>
-      <c r="DG2" s="33"/>
-      <c r="DH2" s="33"/>
-      <c r="DI2" s="33"/>
-      <c r="DJ2" s="33">
+      <c r="CU2" s="38"/>
+      <c r="CV2" s="38"/>
+      <c r="CW2" s="38"/>
+      <c r="CX2" s="38"/>
+      <c r="CY2" s="38"/>
+      <c r="CZ2" s="38"/>
+      <c r="DA2" s="38"/>
+      <c r="DB2" s="38"/>
+      <c r="DC2" s="38"/>
+      <c r="DD2" s="38"/>
+      <c r="DE2" s="38"/>
+      <c r="DF2" s="38"/>
+      <c r="DG2" s="38"/>
+      <c r="DH2" s="38"/>
+      <c r="DI2" s="38"/>
+      <c r="DJ2" s="38">
         <f t="shared" ref="DJ2" si="5">CT2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="DK2" s="33"/>
-      <c r="DL2" s="33"/>
-      <c r="DM2" s="33"/>
-      <c r="DN2" s="33"/>
-      <c r="DO2" s="33"/>
-      <c r="DP2" s="33"/>
-      <c r="DQ2" s="33"/>
-      <c r="DR2" s="33"/>
-      <c r="DS2" s="33"/>
-      <c r="DT2" s="33"/>
-      <c r="DU2" s="33"/>
-      <c r="DV2" s="33"/>
-      <c r="DW2" s="33"/>
-      <c r="DX2" s="33"/>
-      <c r="DY2" s="33"/>
-      <c r="DZ2" s="33">
+      <c r="DK2" s="38"/>
+      <c r="DL2" s="38"/>
+      <c r="DM2" s="38"/>
+      <c r="DN2" s="38"/>
+      <c r="DO2" s="38"/>
+      <c r="DP2" s="38"/>
+      <c r="DQ2" s="38"/>
+      <c r="DR2" s="38"/>
+      <c r="DS2" s="38"/>
+      <c r="DT2" s="38"/>
+      <c r="DU2" s="38"/>
+      <c r="DV2" s="38"/>
+      <c r="DW2" s="38"/>
+      <c r="DX2" s="38"/>
+      <c r="DY2" s="38"/>
+      <c r="DZ2" s="38">
         <f t="shared" ref="DZ2" si="6">DJ2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="EA2" s="33"/>
-      <c r="EB2" s="33"/>
-      <c r="EC2" s="33"/>
-      <c r="ED2" s="33"/>
-      <c r="EE2" s="33"/>
-      <c r="EF2" s="33"/>
-      <c r="EG2" s="33"/>
-      <c r="EH2" s="33"/>
-      <c r="EI2" s="33"/>
-      <c r="EJ2" s="33"/>
-      <c r="EK2" s="33"/>
-      <c r="EL2" s="33"/>
-      <c r="EM2" s="33"/>
-      <c r="EN2" s="33"/>
-      <c r="EO2" s="33"/>
-      <c r="EP2" s="33">
+      <c r="EA2" s="38"/>
+      <c r="EB2" s="38"/>
+      <c r="EC2" s="38"/>
+      <c r="ED2" s="38"/>
+      <c r="EE2" s="38"/>
+      <c r="EF2" s="38"/>
+      <c r="EG2" s="38"/>
+      <c r="EH2" s="38"/>
+      <c r="EI2" s="38"/>
+      <c r="EJ2" s="38"/>
+      <c r="EK2" s="38"/>
+      <c r="EL2" s="38"/>
+      <c r="EM2" s="38"/>
+      <c r="EN2" s="38"/>
+      <c r="EO2" s="38"/>
+      <c r="EP2" s="38">
         <f t="shared" ref="EP2" si="7">DZ2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="EQ2" s="33"/>
-      <c r="ER2" s="33"/>
-      <c r="ES2" s="33"/>
-      <c r="ET2" s="33"/>
-      <c r="EU2" s="33"/>
-      <c r="EV2" s="33"/>
-      <c r="EW2" s="33"/>
-      <c r="EX2" s="33"/>
-      <c r="EY2" s="33"/>
-      <c r="EZ2" s="33"/>
-      <c r="FA2" s="33"/>
-      <c r="FB2" s="33"/>
-      <c r="FC2" s="33"/>
-      <c r="FD2" s="33"/>
-      <c r="FE2" s="33"/>
-      <c r="FF2" s="33">
+      <c r="EQ2" s="38"/>
+      <c r="ER2" s="38"/>
+      <c r="ES2" s="38"/>
+      <c r="ET2" s="38"/>
+      <c r="EU2" s="38"/>
+      <c r="EV2" s="38"/>
+      <c r="EW2" s="38"/>
+      <c r="EX2" s="38"/>
+      <c r="EY2" s="38"/>
+      <c r="EZ2" s="38"/>
+      <c r="FA2" s="38"/>
+      <c r="FB2" s="38"/>
+      <c r="FC2" s="38"/>
+      <c r="FD2" s="38"/>
+      <c r="FE2" s="38"/>
+      <c r="FF2" s="38">
         <f t="shared" ref="FF2" si="8">EP2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="FG2" s="33"/>
-      <c r="FH2" s="33"/>
-      <c r="FI2" s="33"/>
-      <c r="FJ2" s="33"/>
-      <c r="FK2" s="33"/>
-      <c r="FL2" s="33"/>
-      <c r="FM2" s="33"/>
-      <c r="FN2" s="33"/>
-      <c r="FO2" s="33"/>
-      <c r="FP2" s="33"/>
-      <c r="FQ2" s="33"/>
-      <c r="FR2" s="33"/>
-      <c r="FS2" s="33"/>
-      <c r="FT2" s="33"/>
-      <c r="FU2" s="33"/>
-      <c r="FV2" s="33">
+      <c r="FG2" s="38"/>
+      <c r="FH2" s="38"/>
+      <c r="FI2" s="38"/>
+      <c r="FJ2" s="38"/>
+      <c r="FK2" s="38"/>
+      <c r="FL2" s="38"/>
+      <c r="FM2" s="38"/>
+      <c r="FN2" s="38"/>
+      <c r="FO2" s="38"/>
+      <c r="FP2" s="38"/>
+      <c r="FQ2" s="38"/>
+      <c r="FR2" s="38"/>
+      <c r="FS2" s="38"/>
+      <c r="FT2" s="38"/>
+      <c r="FU2" s="38"/>
+      <c r="FV2" s="38">
         <f t="shared" ref="FV2" si="9">FF2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="FW2" s="33"/>
-      <c r="FX2" s="33"/>
-      <c r="FY2" s="33"/>
-      <c r="FZ2" s="33"/>
-      <c r="GA2" s="33"/>
-      <c r="GB2" s="33"/>
-      <c r="GC2" s="33"/>
-      <c r="GD2" s="33"/>
-      <c r="GE2" s="33"/>
-      <c r="GF2" s="33"/>
-      <c r="GG2" s="33"/>
-      <c r="GH2" s="33"/>
-      <c r="GI2" s="33"/>
-      <c r="GJ2" s="33"/>
-      <c r="GK2" s="33"/>
-      <c r="GL2" s="33">
+      <c r="FW2" s="38"/>
+      <c r="FX2" s="38"/>
+      <c r="FY2" s="38"/>
+      <c r="FZ2" s="38"/>
+      <c r="GA2" s="38"/>
+      <c r="GB2" s="38"/>
+      <c r="GC2" s="38"/>
+      <c r="GD2" s="38"/>
+      <c r="GE2" s="38"/>
+      <c r="GF2" s="38"/>
+      <c r="GG2" s="38"/>
+      <c r="GH2" s="38"/>
+      <c r="GI2" s="38"/>
+      <c r="GJ2" s="38"/>
+      <c r="GK2" s="38"/>
+      <c r="GL2" s="38">
         <f t="shared" ref="GL2" si="10">FV2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="GM2" s="33"/>
-      <c r="GN2" s="33"/>
-      <c r="GO2" s="33"/>
-      <c r="GP2" s="33"/>
-      <c r="GQ2" s="33"/>
-      <c r="GR2" s="33"/>
-      <c r="GS2" s="33"/>
-      <c r="GT2" s="33"/>
-      <c r="GU2" s="33"/>
-      <c r="GV2" s="33"/>
-      <c r="GW2" s="33"/>
-      <c r="GX2" s="33"/>
-      <c r="GY2" s="33"/>
-      <c r="GZ2" s="33"/>
-      <c r="HA2" s="33"/>
-      <c r="HB2" s="33">
+      <c r="GM2" s="38"/>
+      <c r="GN2" s="38"/>
+      <c r="GO2" s="38"/>
+      <c r="GP2" s="38"/>
+      <c r="GQ2" s="38"/>
+      <c r="GR2" s="38"/>
+      <c r="GS2" s="38"/>
+      <c r="GT2" s="38"/>
+      <c r="GU2" s="38"/>
+      <c r="GV2" s="38"/>
+      <c r="GW2" s="38"/>
+      <c r="GX2" s="38"/>
+      <c r="GY2" s="38"/>
+      <c r="GZ2" s="38"/>
+      <c r="HA2" s="38"/>
+      <c r="HB2" s="38">
         <f t="shared" ref="HB2" si="11">GL2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="HC2" s="33"/>
-      <c r="HD2" s="33"/>
-      <c r="HE2" s="33"/>
-      <c r="HF2" s="33"/>
-      <c r="HG2" s="33"/>
-      <c r="HH2" s="33"/>
-      <c r="HI2" s="33"/>
-      <c r="HJ2" s="33"/>
-      <c r="HK2" s="33"/>
-      <c r="HL2" s="33"/>
-      <c r="HM2" s="33"/>
-      <c r="HN2" s="33"/>
-      <c r="HO2" s="33"/>
-      <c r="HP2" s="33"/>
-      <c r="HQ2" s="33"/>
-      <c r="HR2" s="33">
+      <c r="HC2" s="38"/>
+      <c r="HD2" s="38"/>
+      <c r="HE2" s="38"/>
+      <c r="HF2" s="38"/>
+      <c r="HG2" s="38"/>
+      <c r="HH2" s="38"/>
+      <c r="HI2" s="38"/>
+      <c r="HJ2" s="38"/>
+      <c r="HK2" s="38"/>
+      <c r="HL2" s="38"/>
+      <c r="HM2" s="38"/>
+      <c r="HN2" s="38"/>
+      <c r="HO2" s="38"/>
+      <c r="HP2" s="38"/>
+      <c r="HQ2" s="38"/>
+      <c r="HR2" s="38">
         <f t="shared" ref="HR2" si="12">HB2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="HS2" s="33"/>
-      <c r="HT2" s="33"/>
-      <c r="HU2" s="33"/>
-      <c r="HV2" s="33"/>
-      <c r="HW2" s="33"/>
-      <c r="HX2" s="33"/>
-      <c r="HY2" s="33"/>
-      <c r="HZ2" s="33"/>
-      <c r="IA2" s="33"/>
-      <c r="IB2" s="33"/>
-      <c r="IC2" s="33"/>
-      <c r="ID2" s="33"/>
-      <c r="IE2" s="33"/>
-      <c r="IF2" s="33"/>
-      <c r="IG2" s="33"/>
-      <c r="IH2" s="33">
+      <c r="HS2" s="38"/>
+      <c r="HT2" s="38"/>
+      <c r="HU2" s="38"/>
+      <c r="HV2" s="38"/>
+      <c r="HW2" s="38"/>
+      <c r="HX2" s="38"/>
+      <c r="HY2" s="38"/>
+      <c r="HZ2" s="38"/>
+      <c r="IA2" s="38"/>
+      <c r="IB2" s="38"/>
+      <c r="IC2" s="38"/>
+      <c r="ID2" s="38"/>
+      <c r="IE2" s="38"/>
+      <c r="IF2" s="38"/>
+      <c r="IG2" s="38"/>
+      <c r="IH2" s="38">
         <f t="shared" ref="IH2" si="13">HR2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="II2" s="33"/>
-      <c r="IJ2" s="33"/>
-      <c r="IK2" s="33"/>
-      <c r="IL2" s="33"/>
-      <c r="IM2" s="33"/>
-      <c r="IN2" s="33"/>
-      <c r="IO2" s="33"/>
-      <c r="IP2" s="33"/>
-      <c r="IQ2" s="33"/>
-      <c r="IR2" s="33"/>
-      <c r="IS2" s="33"/>
-      <c r="IT2" s="33"/>
-      <c r="IU2" s="33"/>
-      <c r="IV2" s="33"/>
-      <c r="IW2" s="33"/>
+      <c r="II2" s="38"/>
+      <c r="IJ2" s="38"/>
+      <c r="IK2" s="38"/>
+      <c r="IL2" s="38"/>
+      <c r="IM2" s="38"/>
+      <c r="IN2" s="38"/>
+      <c r="IO2" s="38"/>
+      <c r="IP2" s="38"/>
+      <c r="IQ2" s="38"/>
+      <c r="IR2" s="38"/>
+      <c r="IS2" s="38"/>
+      <c r="IT2" s="38"/>
+      <c r="IU2" s="38"/>
+      <c r="IV2" s="38"/>
+      <c r="IW2" s="38"/>
     </row>
     <row r="3" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="34">
-        <v>2</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="34">
-        <v>2</v>
-      </c>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="36"/>
-      <c r="AH3" s="34">
-        <v>2</v>
-      </c>
-      <c r="AI3" s="35"/>
-      <c r="AJ3" s="35"/>
-      <c r="AK3" s="35"/>
-      <c r="AL3" s="35"/>
-      <c r="AM3" s="35"/>
-      <c r="AN3" s="35"/>
-      <c r="AO3" s="35"/>
-      <c r="AP3" s="35"/>
-      <c r="AQ3" s="35"/>
-      <c r="AR3" s="35"/>
-      <c r="AS3" s="35"/>
-      <c r="AT3" s="35"/>
-      <c r="AU3" s="35"/>
-      <c r="AV3" s="35"/>
-      <c r="AW3" s="36"/>
-      <c r="AX3" s="34">
-        <v>2</v>
-      </c>
-      <c r="AY3" s="35"/>
-      <c r="AZ3" s="35"/>
-      <c r="BA3" s="35"/>
-      <c r="BB3" s="35"/>
-      <c r="BC3" s="35"/>
-      <c r="BD3" s="35"/>
-      <c r="BE3" s="35"/>
-      <c r="BF3" s="35"/>
-      <c r="BG3" s="35"/>
-      <c r="BH3" s="35"/>
-      <c r="BI3" s="35"/>
-      <c r="BJ3" s="35"/>
-      <c r="BK3" s="35"/>
-      <c r="BL3" s="35"/>
-      <c r="BM3" s="36"/>
-      <c r="BN3" s="34">
-        <v>6</v>
-      </c>
-      <c r="BO3" s="35"/>
-      <c r="BP3" s="35"/>
-      <c r="BQ3" s="35"/>
-      <c r="BR3" s="35"/>
-      <c r="BS3" s="35"/>
-      <c r="BT3" s="35"/>
-      <c r="BU3" s="35"/>
-      <c r="BV3" s="35"/>
-      <c r="BW3" s="35"/>
-      <c r="BX3" s="35"/>
-      <c r="BY3" s="35"/>
-      <c r="BZ3" s="35"/>
-      <c r="CA3" s="35"/>
-      <c r="CB3" s="35"/>
-      <c r="CC3" s="36"/>
-      <c r="CD3" s="34">
-        <v>6</v>
-      </c>
-      <c r="CE3" s="35"/>
-      <c r="CF3" s="35"/>
-      <c r="CG3" s="35"/>
-      <c r="CH3" s="35"/>
-      <c r="CI3" s="35"/>
-      <c r="CJ3" s="35"/>
-      <c r="CK3" s="35"/>
-      <c r="CL3" s="35"/>
-      <c r="CM3" s="35"/>
-      <c r="CN3" s="35"/>
-      <c r="CO3" s="35"/>
-      <c r="CP3" s="35"/>
-      <c r="CQ3" s="35"/>
-      <c r="CR3" s="35"/>
-      <c r="CS3" s="36"/>
-      <c r="CT3" s="34">
-        <v>6</v>
-      </c>
-      <c r="CU3" s="35"/>
-      <c r="CV3" s="35"/>
-      <c r="CW3" s="35"/>
-      <c r="CX3" s="35"/>
-      <c r="CY3" s="35"/>
-      <c r="CZ3" s="35"/>
-      <c r="DA3" s="35"/>
-      <c r="DB3" s="35"/>
-      <c r="DC3" s="35"/>
-      <c r="DD3" s="35"/>
-      <c r="DE3" s="35"/>
-      <c r="DF3" s="35"/>
-      <c r="DG3" s="35"/>
-      <c r="DH3" s="35"/>
-      <c r="DI3" s="36"/>
-      <c r="DJ3" s="34">
-        <v>6</v>
-      </c>
-      <c r="DK3" s="35"/>
-      <c r="DL3" s="35"/>
-      <c r="DM3" s="35"/>
-      <c r="DN3" s="35"/>
-      <c r="DO3" s="35"/>
-      <c r="DP3" s="35"/>
-      <c r="DQ3" s="35"/>
-      <c r="DR3" s="35"/>
-      <c r="DS3" s="35"/>
-      <c r="DT3" s="35"/>
-      <c r="DU3" s="35"/>
-      <c r="DV3" s="35"/>
-      <c r="DW3" s="35"/>
-      <c r="DX3" s="35"/>
-      <c r="DY3" s="36"/>
-      <c r="DZ3" s="42">
-        <v>10</v>
-      </c>
-      <c r="EA3" s="40"/>
-      <c r="EB3" s="40"/>
-      <c r="EC3" s="40"/>
-      <c r="ED3" s="40"/>
-      <c r="EE3" s="40"/>
-      <c r="EF3" s="40"/>
-      <c r="EG3" s="40"/>
-      <c r="EH3" s="40"/>
-      <c r="EI3" s="40"/>
-      <c r="EJ3" s="40"/>
-      <c r="EK3" s="40"/>
-      <c r="EL3" s="40"/>
-      <c r="EM3" s="40"/>
-      <c r="EN3" s="40"/>
-      <c r="EO3" s="41"/>
-      <c r="EP3" s="39">
-        <v>10</v>
-      </c>
-      <c r="EQ3" s="40"/>
-      <c r="ER3" s="40"/>
-      <c r="ES3" s="40"/>
-      <c r="ET3" s="40"/>
-      <c r="EU3" s="40"/>
-      <c r="EV3" s="40"/>
-      <c r="EW3" s="40"/>
-      <c r="EX3" s="40"/>
-      <c r="EY3" s="40"/>
-      <c r="EZ3" s="40"/>
-      <c r="FA3" s="40"/>
-      <c r="FB3" s="40"/>
-      <c r="FC3" s="40"/>
-      <c r="FD3" s="40"/>
-      <c r="FE3" s="41"/>
-      <c r="FF3" s="39">
-        <v>10</v>
-      </c>
-      <c r="FG3" s="40"/>
-      <c r="FH3" s="40"/>
-      <c r="FI3" s="40"/>
-      <c r="FJ3" s="40"/>
-      <c r="FK3" s="40"/>
-      <c r="FL3" s="40"/>
-      <c r="FM3" s="40"/>
-      <c r="FN3" s="40"/>
-      <c r="FO3" s="40"/>
-      <c r="FP3" s="40"/>
-      <c r="FQ3" s="40"/>
-      <c r="FR3" s="40"/>
-      <c r="FS3" s="40"/>
-      <c r="FT3" s="40"/>
-      <c r="FU3" s="41"/>
-      <c r="FV3" s="39">
-        <v>10</v>
-      </c>
-      <c r="FW3" s="40"/>
-      <c r="FX3" s="40"/>
-      <c r="FY3" s="40"/>
-      <c r="FZ3" s="40"/>
-      <c r="GA3" s="40"/>
-      <c r="GB3" s="40"/>
-      <c r="GC3" s="40"/>
-      <c r="GD3" s="40"/>
-      <c r="GE3" s="40"/>
-      <c r="GF3" s="40"/>
-      <c r="GG3" s="40"/>
-      <c r="GH3" s="40"/>
-      <c r="GI3" s="40"/>
-      <c r="GJ3" s="40"/>
-      <c r="GK3" s="41"/>
-      <c r="GL3" s="39">
-        <v>14</v>
-      </c>
-      <c r="GM3" s="40"/>
-      <c r="GN3" s="40"/>
-      <c r="GO3" s="40"/>
-      <c r="GP3" s="40"/>
-      <c r="GQ3" s="40"/>
-      <c r="GR3" s="40"/>
-      <c r="GS3" s="40"/>
-      <c r="GT3" s="40"/>
-      <c r="GU3" s="40"/>
-      <c r="GV3" s="40"/>
-      <c r="GW3" s="40"/>
-      <c r="GX3" s="40"/>
-      <c r="GY3" s="40"/>
-      <c r="GZ3" s="40"/>
-      <c r="HA3" s="41"/>
-      <c r="HB3" s="39">
-        <v>14</v>
-      </c>
-      <c r="HC3" s="40"/>
-      <c r="HD3" s="40"/>
-      <c r="HE3" s="40"/>
-      <c r="HF3" s="40"/>
-      <c r="HG3" s="40"/>
-      <c r="HH3" s="40"/>
-      <c r="HI3" s="40"/>
-      <c r="HJ3" s="40"/>
-      <c r="HK3" s="40"/>
-      <c r="HL3" s="40"/>
-      <c r="HM3" s="40"/>
-      <c r="HN3" s="40"/>
-      <c r="HO3" s="40"/>
-      <c r="HP3" s="40"/>
-      <c r="HQ3" s="41"/>
-      <c r="HR3" s="39">
-        <v>14</v>
-      </c>
-      <c r="HS3" s="40"/>
-      <c r="HT3" s="40"/>
-      <c r="HU3" s="40"/>
-      <c r="HV3" s="40"/>
-      <c r="HW3" s="40"/>
-      <c r="HX3" s="40"/>
-      <c r="HY3" s="40"/>
-      <c r="HZ3" s="40"/>
-      <c r="IA3" s="40"/>
-      <c r="IB3" s="40"/>
-      <c r="IC3" s="40"/>
-      <c r="ID3" s="40"/>
-      <c r="IE3" s="40"/>
-      <c r="IF3" s="40"/>
-      <c r="IG3" s="41"/>
-      <c r="IH3" s="39">
-        <v>14</v>
-      </c>
-      <c r="II3" s="40"/>
-      <c r="IJ3" s="40"/>
-      <c r="IK3" s="40"/>
-      <c r="IL3" s="40"/>
-      <c r="IM3" s="40"/>
-      <c r="IN3" s="40"/>
-      <c r="IO3" s="40"/>
-      <c r="IP3" s="40"/>
-      <c r="IQ3" s="40"/>
-      <c r="IR3" s="40"/>
-      <c r="IS3" s="40"/>
-      <c r="IT3" s="40"/>
-      <c r="IU3" s="40"/>
-      <c r="IV3" s="40"/>
-      <c r="IW3" s="41"/>
+      <c r="B3" s="39">
+        <v>5</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="39">
+        <v>5</v>
+      </c>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="40"/>
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="41"/>
+      <c r="AH3" s="39">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="40"/>
+      <c r="AK3" s="40"/>
+      <c r="AL3" s="40"/>
+      <c r="AM3" s="40"/>
+      <c r="AN3" s="40"/>
+      <c r="AO3" s="40"/>
+      <c r="AP3" s="40"/>
+      <c r="AQ3" s="40"/>
+      <c r="AR3" s="40"/>
+      <c r="AS3" s="40"/>
+      <c r="AT3" s="40"/>
+      <c r="AU3" s="40"/>
+      <c r="AV3" s="40"/>
+      <c r="AW3" s="41"/>
+      <c r="AX3" s="39">
+        <v>5</v>
+      </c>
+      <c r="AY3" s="40"/>
+      <c r="AZ3" s="40"/>
+      <c r="BA3" s="40"/>
+      <c r="BB3" s="40"/>
+      <c r="BC3" s="40"/>
+      <c r="BD3" s="40"/>
+      <c r="BE3" s="40"/>
+      <c r="BF3" s="40"/>
+      <c r="BG3" s="40"/>
+      <c r="BH3" s="40"/>
+      <c r="BI3" s="40"/>
+      <c r="BJ3" s="40"/>
+      <c r="BK3" s="40"/>
+      <c r="BL3" s="40"/>
+      <c r="BM3" s="41"/>
+      <c r="BN3" s="39">
+        <v>9</v>
+      </c>
+      <c r="BO3" s="40"/>
+      <c r="BP3" s="40"/>
+      <c r="BQ3" s="40"/>
+      <c r="BR3" s="40"/>
+      <c r="BS3" s="40"/>
+      <c r="BT3" s="40"/>
+      <c r="BU3" s="40"/>
+      <c r="BV3" s="40"/>
+      <c r="BW3" s="40"/>
+      <c r="BX3" s="40"/>
+      <c r="BY3" s="40"/>
+      <c r="BZ3" s="40"/>
+      <c r="CA3" s="40"/>
+      <c r="CB3" s="40"/>
+      <c r="CC3" s="41"/>
+      <c r="CD3" s="39">
+        <v>9</v>
+      </c>
+      <c r="CE3" s="40"/>
+      <c r="CF3" s="40"/>
+      <c r="CG3" s="40"/>
+      <c r="CH3" s="40"/>
+      <c r="CI3" s="40"/>
+      <c r="CJ3" s="40"/>
+      <c r="CK3" s="40"/>
+      <c r="CL3" s="40"/>
+      <c r="CM3" s="40"/>
+      <c r="CN3" s="40"/>
+      <c r="CO3" s="40"/>
+      <c r="CP3" s="40"/>
+      <c r="CQ3" s="40"/>
+      <c r="CR3" s="40"/>
+      <c r="CS3" s="41"/>
+      <c r="CT3" s="39">
+        <v>9</v>
+      </c>
+      <c r="CU3" s="40"/>
+      <c r="CV3" s="40"/>
+      <c r="CW3" s="40"/>
+      <c r="CX3" s="40"/>
+      <c r="CY3" s="40"/>
+      <c r="CZ3" s="40"/>
+      <c r="DA3" s="40"/>
+      <c r="DB3" s="40"/>
+      <c r="DC3" s="40"/>
+      <c r="DD3" s="40"/>
+      <c r="DE3" s="40"/>
+      <c r="DF3" s="40"/>
+      <c r="DG3" s="40"/>
+      <c r="DH3" s="40"/>
+      <c r="DI3" s="41"/>
+      <c r="DJ3" s="39">
+        <v>9</v>
+      </c>
+      <c r="DK3" s="40"/>
+      <c r="DL3" s="40"/>
+      <c r="DM3" s="40"/>
+      <c r="DN3" s="40"/>
+      <c r="DO3" s="40"/>
+      <c r="DP3" s="40"/>
+      <c r="DQ3" s="40"/>
+      <c r="DR3" s="40"/>
+      <c r="DS3" s="40"/>
+      <c r="DT3" s="40"/>
+      <c r="DU3" s="40"/>
+      <c r="DV3" s="40"/>
+      <c r="DW3" s="40"/>
+      <c r="DX3" s="40"/>
+      <c r="DY3" s="41"/>
+      <c r="DZ3" s="44">
+        <v>13</v>
+      </c>
+      <c r="EA3" s="45"/>
+      <c r="EB3" s="45"/>
+      <c r="EC3" s="45"/>
+      <c r="ED3" s="45"/>
+      <c r="EE3" s="45"/>
+      <c r="EF3" s="45"/>
+      <c r="EG3" s="45"/>
+      <c r="EH3" s="45"/>
+      <c r="EI3" s="45"/>
+      <c r="EJ3" s="45"/>
+      <c r="EK3" s="45"/>
+      <c r="EL3" s="45"/>
+      <c r="EM3" s="45"/>
+      <c r="EN3" s="45"/>
+      <c r="EO3" s="46"/>
+      <c r="EP3" s="47">
+        <v>13</v>
+      </c>
+      <c r="EQ3" s="45"/>
+      <c r="ER3" s="45"/>
+      <c r="ES3" s="45"/>
+      <c r="ET3" s="45"/>
+      <c r="EU3" s="45"/>
+      <c r="EV3" s="45"/>
+      <c r="EW3" s="45"/>
+      <c r="EX3" s="45"/>
+      <c r="EY3" s="45"/>
+      <c r="EZ3" s="45"/>
+      <c r="FA3" s="45"/>
+      <c r="FB3" s="45"/>
+      <c r="FC3" s="45"/>
+      <c r="FD3" s="45"/>
+      <c r="FE3" s="46"/>
+      <c r="FF3" s="47">
+        <v>13</v>
+      </c>
+      <c r="FG3" s="45"/>
+      <c r="FH3" s="45"/>
+      <c r="FI3" s="45"/>
+      <c r="FJ3" s="45"/>
+      <c r="FK3" s="45"/>
+      <c r="FL3" s="45"/>
+      <c r="FM3" s="45"/>
+      <c r="FN3" s="45"/>
+      <c r="FO3" s="45"/>
+      <c r="FP3" s="45"/>
+      <c r="FQ3" s="45"/>
+      <c r="FR3" s="45"/>
+      <c r="FS3" s="45"/>
+      <c r="FT3" s="45"/>
+      <c r="FU3" s="46"/>
+      <c r="FV3" s="47">
+        <v>13</v>
+      </c>
+      <c r="FW3" s="45"/>
+      <c r="FX3" s="45"/>
+      <c r="FY3" s="45"/>
+      <c r="FZ3" s="45"/>
+      <c r="GA3" s="45"/>
+      <c r="GB3" s="45"/>
+      <c r="GC3" s="45"/>
+      <c r="GD3" s="45"/>
+      <c r="GE3" s="45"/>
+      <c r="GF3" s="45"/>
+      <c r="GG3" s="45"/>
+      <c r="GH3" s="45"/>
+      <c r="GI3" s="45"/>
+      <c r="GJ3" s="45"/>
+      <c r="GK3" s="46"/>
+      <c r="GL3" s="47">
+        <v>17</v>
+      </c>
+      <c r="GM3" s="45"/>
+      <c r="GN3" s="45"/>
+      <c r="GO3" s="45"/>
+      <c r="GP3" s="45"/>
+      <c r="GQ3" s="45"/>
+      <c r="GR3" s="45"/>
+      <c r="GS3" s="45"/>
+      <c r="GT3" s="45"/>
+      <c r="GU3" s="45"/>
+      <c r="GV3" s="45"/>
+      <c r="GW3" s="45"/>
+      <c r="GX3" s="45"/>
+      <c r="GY3" s="45"/>
+      <c r="GZ3" s="45"/>
+      <c r="HA3" s="46"/>
+      <c r="HB3" s="47">
+        <v>17</v>
+      </c>
+      <c r="HC3" s="45"/>
+      <c r="HD3" s="45"/>
+      <c r="HE3" s="45"/>
+      <c r="HF3" s="45"/>
+      <c r="HG3" s="45"/>
+      <c r="HH3" s="45"/>
+      <c r="HI3" s="45"/>
+      <c r="HJ3" s="45"/>
+      <c r="HK3" s="45"/>
+      <c r="HL3" s="45"/>
+      <c r="HM3" s="45"/>
+      <c r="HN3" s="45"/>
+      <c r="HO3" s="45"/>
+      <c r="HP3" s="45"/>
+      <c r="HQ3" s="46"/>
+      <c r="HR3" s="47">
+        <v>17</v>
+      </c>
+      <c r="HS3" s="45"/>
+      <c r="HT3" s="45"/>
+      <c r="HU3" s="45"/>
+      <c r="HV3" s="45"/>
+      <c r="HW3" s="45"/>
+      <c r="HX3" s="45"/>
+      <c r="HY3" s="45"/>
+      <c r="HZ3" s="45"/>
+      <c r="IA3" s="45"/>
+      <c r="IB3" s="45"/>
+      <c r="IC3" s="45"/>
+      <c r="ID3" s="45"/>
+      <c r="IE3" s="45"/>
+      <c r="IF3" s="45"/>
+      <c r="IG3" s="46"/>
+      <c r="IH3" s="47">
+        <v>17</v>
+      </c>
+      <c r="II3" s="45"/>
+      <c r="IJ3" s="45"/>
+      <c r="IK3" s="45"/>
+      <c r="IL3" s="45"/>
+      <c r="IM3" s="45"/>
+      <c r="IN3" s="45"/>
+      <c r="IO3" s="45"/>
+      <c r="IP3" s="45"/>
+      <c r="IQ3" s="45"/>
+      <c r="IR3" s="45"/>
+      <c r="IS3" s="45"/>
+      <c r="IT3" s="45"/>
+      <c r="IU3" s="45"/>
+      <c r="IV3" s="45"/>
+      <c r="IW3" s="46"/>
     </row>
     <row r="4" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="37" t="s">
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="38" t="s">
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="37" t="s">
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AI4" s="37"/>
-      <c r="AJ4" s="37"/>
-      <c r="AK4" s="37"/>
-      <c r="AL4" s="37"/>
-      <c r="AM4" s="37"/>
-      <c r="AN4" s="37"/>
-      <c r="AO4" s="37"/>
-      <c r="AP4" s="38" t="s">
+      <c r="AI4" s="42"/>
+      <c r="AJ4" s="42"/>
+      <c r="AK4" s="42"/>
+      <c r="AL4" s="42"/>
+      <c r="AM4" s="42"/>
+      <c r="AN4" s="42"/>
+      <c r="AO4" s="42"/>
+      <c r="AP4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AQ4" s="38"/>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="38"/>
-      <c r="AU4" s="38"/>
-      <c r="AV4" s="38"/>
-      <c r="AW4" s="38"/>
-      <c r="AX4" s="37" t="s">
+      <c r="AQ4" s="43"/>
+      <c r="AR4" s="43"/>
+      <c r="AS4" s="43"/>
+      <c r="AT4" s="43"/>
+      <c r="AU4" s="43"/>
+      <c r="AV4" s="43"/>
+      <c r="AW4" s="43"/>
+      <c r="AX4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AY4" s="37"/>
-      <c r="AZ4" s="37"/>
-      <c r="BA4" s="37"/>
-      <c r="BB4" s="37"/>
-      <c r="BC4" s="37"/>
-      <c r="BD4" s="37"/>
-      <c r="BE4" s="37"/>
-      <c r="BF4" s="38" t="s">
+      <c r="AY4" s="42"/>
+      <c r="AZ4" s="42"/>
+      <c r="BA4" s="42"/>
+      <c r="BB4" s="42"/>
+      <c r="BC4" s="42"/>
+      <c r="BD4" s="42"/>
+      <c r="BE4" s="42"/>
+      <c r="BF4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="BG4" s="38"/>
-      <c r="BH4" s="38"/>
-      <c r="BI4" s="38"/>
-      <c r="BJ4" s="38"/>
-      <c r="BK4" s="38"/>
-      <c r="BL4" s="38"/>
-      <c r="BM4" s="38"/>
-      <c r="BN4" s="37" t="s">
+      <c r="BG4" s="43"/>
+      <c r="BH4" s="43"/>
+      <c r="BI4" s="43"/>
+      <c r="BJ4" s="43"/>
+      <c r="BK4" s="43"/>
+      <c r="BL4" s="43"/>
+      <c r="BM4" s="43"/>
+      <c r="BN4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="BO4" s="37"/>
-      <c r="BP4" s="37"/>
-      <c r="BQ4" s="37"/>
-      <c r="BR4" s="37"/>
-      <c r="BS4" s="37"/>
-      <c r="BT4" s="37"/>
-      <c r="BU4" s="37"/>
-      <c r="BV4" s="38" t="s">
+      <c r="BO4" s="42"/>
+      <c r="BP4" s="42"/>
+      <c r="BQ4" s="42"/>
+      <c r="BR4" s="42"/>
+      <c r="BS4" s="42"/>
+      <c r="BT4" s="42"/>
+      <c r="BU4" s="42"/>
+      <c r="BV4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="BW4" s="38"/>
-      <c r="BX4" s="38"/>
-      <c r="BY4" s="38"/>
-      <c r="BZ4" s="38"/>
-      <c r="CA4" s="38"/>
-      <c r="CB4" s="38"/>
-      <c r="CC4" s="38"/>
-      <c r="CD4" s="37" t="s">
+      <c r="BW4" s="43"/>
+      <c r="BX4" s="43"/>
+      <c r="BY4" s="43"/>
+      <c r="BZ4" s="43"/>
+      <c r="CA4" s="43"/>
+      <c r="CB4" s="43"/>
+      <c r="CC4" s="43"/>
+      <c r="CD4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="CE4" s="37"/>
-      <c r="CF4" s="37"/>
-      <c r="CG4" s="37"/>
-      <c r="CH4" s="37"/>
-      <c r="CI4" s="37"/>
-      <c r="CJ4" s="37"/>
-      <c r="CK4" s="37"/>
-      <c r="CL4" s="38" t="s">
+      <c r="CE4" s="42"/>
+      <c r="CF4" s="42"/>
+      <c r="CG4" s="42"/>
+      <c r="CH4" s="42"/>
+      <c r="CI4" s="42"/>
+      <c r="CJ4" s="42"/>
+      <c r="CK4" s="42"/>
+      <c r="CL4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="CM4" s="38"/>
-      <c r="CN4" s="38"/>
-      <c r="CO4" s="38"/>
-      <c r="CP4" s="38"/>
-      <c r="CQ4" s="38"/>
-      <c r="CR4" s="38"/>
-      <c r="CS4" s="38"/>
-      <c r="CT4" s="37" t="s">
+      <c r="CM4" s="43"/>
+      <c r="CN4" s="43"/>
+      <c r="CO4" s="43"/>
+      <c r="CP4" s="43"/>
+      <c r="CQ4" s="43"/>
+      <c r="CR4" s="43"/>
+      <c r="CS4" s="43"/>
+      <c r="CT4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="CU4" s="37"/>
-      <c r="CV4" s="37"/>
-      <c r="CW4" s="37"/>
-      <c r="CX4" s="37"/>
-      <c r="CY4" s="37"/>
-      <c r="CZ4" s="37"/>
-      <c r="DA4" s="37"/>
-      <c r="DB4" s="38" t="s">
+      <c r="CU4" s="42"/>
+      <c r="CV4" s="42"/>
+      <c r="CW4" s="42"/>
+      <c r="CX4" s="42"/>
+      <c r="CY4" s="42"/>
+      <c r="CZ4" s="42"/>
+      <c r="DA4" s="42"/>
+      <c r="DB4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="DC4" s="38"/>
-      <c r="DD4" s="38"/>
-      <c r="DE4" s="38"/>
-      <c r="DF4" s="38"/>
-      <c r="DG4" s="38"/>
-      <c r="DH4" s="38"/>
-      <c r="DI4" s="38"/>
-      <c r="DJ4" s="37" t="s">
+      <c r="DC4" s="43"/>
+      <c r="DD4" s="43"/>
+      <c r="DE4" s="43"/>
+      <c r="DF4" s="43"/>
+      <c r="DG4" s="43"/>
+      <c r="DH4" s="43"/>
+      <c r="DI4" s="43"/>
+      <c r="DJ4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="DK4" s="37"/>
-      <c r="DL4" s="37"/>
-      <c r="DM4" s="37"/>
-      <c r="DN4" s="37"/>
-      <c r="DO4" s="37"/>
-      <c r="DP4" s="37"/>
-      <c r="DQ4" s="37"/>
-      <c r="DR4" s="38" t="s">
+      <c r="DK4" s="42"/>
+      <c r="DL4" s="42"/>
+      <c r="DM4" s="42"/>
+      <c r="DN4" s="42"/>
+      <c r="DO4" s="42"/>
+      <c r="DP4" s="42"/>
+      <c r="DQ4" s="42"/>
+      <c r="DR4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="DS4" s="38"/>
-      <c r="DT4" s="38"/>
-      <c r="DU4" s="38"/>
-      <c r="DV4" s="38"/>
-      <c r="DW4" s="38"/>
-      <c r="DX4" s="38"/>
-      <c r="DY4" s="38"/>
-      <c r="DZ4" s="37" t="s">
+      <c r="DS4" s="43"/>
+      <c r="DT4" s="43"/>
+      <c r="DU4" s="43"/>
+      <c r="DV4" s="43"/>
+      <c r="DW4" s="43"/>
+      <c r="DX4" s="43"/>
+      <c r="DY4" s="43"/>
+      <c r="DZ4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="EA4" s="37"/>
-      <c r="EB4" s="37"/>
-      <c r="EC4" s="37"/>
-      <c r="ED4" s="37"/>
-      <c r="EE4" s="37"/>
-      <c r="EF4" s="37"/>
-      <c r="EG4" s="37"/>
-      <c r="EH4" s="38" t="s">
+      <c r="EA4" s="42"/>
+      <c r="EB4" s="42"/>
+      <c r="EC4" s="42"/>
+      <c r="ED4" s="42"/>
+      <c r="EE4" s="42"/>
+      <c r="EF4" s="42"/>
+      <c r="EG4" s="42"/>
+      <c r="EH4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="EI4" s="38"/>
-      <c r="EJ4" s="38"/>
-      <c r="EK4" s="38"/>
-      <c r="EL4" s="38"/>
-      <c r="EM4" s="38"/>
-      <c r="EN4" s="38"/>
-      <c r="EO4" s="38"/>
-      <c r="EP4" s="37" t="s">
+      <c r="EI4" s="43"/>
+      <c r="EJ4" s="43"/>
+      <c r="EK4" s="43"/>
+      <c r="EL4" s="43"/>
+      <c r="EM4" s="43"/>
+      <c r="EN4" s="43"/>
+      <c r="EO4" s="43"/>
+      <c r="EP4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="EQ4" s="37"/>
-      <c r="ER4" s="37"/>
-      <c r="ES4" s="37"/>
-      <c r="ET4" s="37"/>
-      <c r="EU4" s="37"/>
-      <c r="EV4" s="37"/>
-      <c r="EW4" s="37"/>
-      <c r="EX4" s="38" t="s">
+      <c r="EQ4" s="42"/>
+      <c r="ER4" s="42"/>
+      <c r="ES4" s="42"/>
+      <c r="ET4" s="42"/>
+      <c r="EU4" s="42"/>
+      <c r="EV4" s="42"/>
+      <c r="EW4" s="42"/>
+      <c r="EX4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="EY4" s="38"/>
-      <c r="EZ4" s="38"/>
-      <c r="FA4" s="38"/>
-      <c r="FB4" s="38"/>
-      <c r="FC4" s="38"/>
-      <c r="FD4" s="38"/>
-      <c r="FE4" s="38"/>
-      <c r="FF4" s="37" t="s">
+      <c r="EY4" s="43"/>
+      <c r="EZ4" s="43"/>
+      <c r="FA4" s="43"/>
+      <c r="FB4" s="43"/>
+      <c r="FC4" s="43"/>
+      <c r="FD4" s="43"/>
+      <c r="FE4" s="43"/>
+      <c r="FF4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="FG4" s="37"/>
-      <c r="FH4" s="37"/>
-      <c r="FI4" s="37"/>
-      <c r="FJ4" s="37"/>
-      <c r="FK4" s="37"/>
-      <c r="FL4" s="37"/>
-      <c r="FM4" s="37"/>
-      <c r="FN4" s="38" t="s">
+      <c r="FG4" s="42"/>
+      <c r="FH4" s="42"/>
+      <c r="FI4" s="42"/>
+      <c r="FJ4" s="42"/>
+      <c r="FK4" s="42"/>
+      <c r="FL4" s="42"/>
+      <c r="FM4" s="42"/>
+      <c r="FN4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="FO4" s="38"/>
-      <c r="FP4" s="38"/>
-      <c r="FQ4" s="38"/>
-      <c r="FR4" s="38"/>
-      <c r="FS4" s="38"/>
-      <c r="FT4" s="38"/>
-      <c r="FU4" s="38"/>
-      <c r="FV4" s="37" t="s">
+      <c r="FO4" s="43"/>
+      <c r="FP4" s="43"/>
+      <c r="FQ4" s="43"/>
+      <c r="FR4" s="43"/>
+      <c r="FS4" s="43"/>
+      <c r="FT4" s="43"/>
+      <c r="FU4" s="43"/>
+      <c r="FV4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="FW4" s="37"/>
-      <c r="FX4" s="37"/>
-      <c r="FY4" s="37"/>
-      <c r="FZ4" s="37"/>
-      <c r="GA4" s="37"/>
-      <c r="GB4" s="37"/>
-      <c r="GC4" s="37"/>
-      <c r="GD4" s="38" t="s">
+      <c r="FW4" s="42"/>
+      <c r="FX4" s="42"/>
+      <c r="FY4" s="42"/>
+      <c r="FZ4" s="42"/>
+      <c r="GA4" s="42"/>
+      <c r="GB4" s="42"/>
+      <c r="GC4" s="42"/>
+      <c r="GD4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="GE4" s="38"/>
-      <c r="GF4" s="38"/>
-      <c r="GG4" s="38"/>
-      <c r="GH4" s="38"/>
-      <c r="GI4" s="38"/>
-      <c r="GJ4" s="38"/>
-      <c r="GK4" s="38"/>
-      <c r="GL4" s="37" t="s">
+      <c r="GE4" s="43"/>
+      <c r="GF4" s="43"/>
+      <c r="GG4" s="43"/>
+      <c r="GH4" s="43"/>
+      <c r="GI4" s="43"/>
+      <c r="GJ4" s="43"/>
+      <c r="GK4" s="43"/>
+      <c r="GL4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="GM4" s="37"/>
-      <c r="GN4" s="37"/>
-      <c r="GO4" s="37"/>
-      <c r="GP4" s="37"/>
-      <c r="GQ4" s="37"/>
-      <c r="GR4" s="37"/>
-      <c r="GS4" s="37"/>
-      <c r="GT4" s="38" t="s">
+      <c r="GM4" s="42"/>
+      <c r="GN4" s="42"/>
+      <c r="GO4" s="42"/>
+      <c r="GP4" s="42"/>
+      <c r="GQ4" s="42"/>
+      <c r="GR4" s="42"/>
+      <c r="GS4" s="42"/>
+      <c r="GT4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="GU4" s="38"/>
-      <c r="GV4" s="38"/>
-      <c r="GW4" s="38"/>
-      <c r="GX4" s="38"/>
-      <c r="GY4" s="38"/>
-      <c r="GZ4" s="38"/>
-      <c r="HA4" s="38"/>
-      <c r="HB4" s="37" t="s">
+      <c r="GU4" s="43"/>
+      <c r="GV4" s="43"/>
+      <c r="GW4" s="43"/>
+      <c r="GX4" s="43"/>
+      <c r="GY4" s="43"/>
+      <c r="GZ4" s="43"/>
+      <c r="HA4" s="43"/>
+      <c r="HB4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="HC4" s="37"/>
-      <c r="HD4" s="37"/>
-      <c r="HE4" s="37"/>
-      <c r="HF4" s="37"/>
-      <c r="HG4" s="37"/>
-      <c r="HH4" s="37"/>
-      <c r="HI4" s="37"/>
-      <c r="HJ4" s="38" t="s">
+      <c r="HC4" s="42"/>
+      <c r="HD4" s="42"/>
+      <c r="HE4" s="42"/>
+      <c r="HF4" s="42"/>
+      <c r="HG4" s="42"/>
+      <c r="HH4" s="42"/>
+      <c r="HI4" s="42"/>
+      <c r="HJ4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="HK4" s="38"/>
-      <c r="HL4" s="38"/>
-      <c r="HM4" s="38"/>
-      <c r="HN4" s="38"/>
-      <c r="HO4" s="38"/>
-      <c r="HP4" s="38"/>
-      <c r="HQ4" s="38"/>
-      <c r="HR4" s="37" t="s">
+      <c r="HK4" s="43"/>
+      <c r="HL4" s="43"/>
+      <c r="HM4" s="43"/>
+      <c r="HN4" s="43"/>
+      <c r="HO4" s="43"/>
+      <c r="HP4" s="43"/>
+      <c r="HQ4" s="43"/>
+      <c r="HR4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="HS4" s="37"/>
-      <c r="HT4" s="37"/>
-      <c r="HU4" s="37"/>
-      <c r="HV4" s="37"/>
-      <c r="HW4" s="37"/>
-      <c r="HX4" s="37"/>
-      <c r="HY4" s="37"/>
-      <c r="HZ4" s="38" t="s">
+      <c r="HS4" s="42"/>
+      <c r="HT4" s="42"/>
+      <c r="HU4" s="42"/>
+      <c r="HV4" s="42"/>
+      <c r="HW4" s="42"/>
+      <c r="HX4" s="42"/>
+      <c r="HY4" s="42"/>
+      <c r="HZ4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="IA4" s="38"/>
-      <c r="IB4" s="38"/>
-      <c r="IC4" s="38"/>
-      <c r="ID4" s="38"/>
-      <c r="IE4" s="38"/>
-      <c r="IF4" s="38"/>
-      <c r="IG4" s="38"/>
-      <c r="IH4" s="37" t="s">
+      <c r="IA4" s="43"/>
+      <c r="IB4" s="43"/>
+      <c r="IC4" s="43"/>
+      <c r="ID4" s="43"/>
+      <c r="IE4" s="43"/>
+      <c r="IF4" s="43"/>
+      <c r="IG4" s="43"/>
+      <c r="IH4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="II4" s="37"/>
-      <c r="IJ4" s="37"/>
-      <c r="IK4" s="37"/>
-      <c r="IL4" s="37"/>
-      <c r="IM4" s="37"/>
-      <c r="IN4" s="37"/>
-      <c r="IO4" s="37"/>
-      <c r="IP4" s="38" t="s">
+      <c r="II4" s="42"/>
+      <c r="IJ4" s="42"/>
+      <c r="IK4" s="42"/>
+      <c r="IL4" s="42"/>
+      <c r="IM4" s="42"/>
+      <c r="IN4" s="42"/>
+      <c r="IO4" s="42"/>
+      <c r="IP4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="IQ4" s="38"/>
-      <c r="IR4" s="38"/>
-      <c r="IS4" s="38"/>
-      <c r="IT4" s="38"/>
-      <c r="IU4" s="38"/>
-      <c r="IV4" s="38"/>
-      <c r="IW4" s="38"/>
+      <c r="IQ4" s="43"/>
+      <c r="IR4" s="43"/>
+      <c r="IS4" s="43"/>
+      <c r="IT4" s="43"/>
+      <c r="IU4" s="43"/>
+      <c r="IV4" s="43"/>
+      <c r="IW4" s="43"/>
     </row>
     <row r="5" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -27127,41 +27257,35 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="R3:AG3"/>
-    <mergeCell ref="AH4:AO4"/>
-    <mergeCell ref="AP4:AW4"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="BF4:BM4"/>
-    <mergeCell ref="BN4:BU4"/>
-    <mergeCell ref="BV4:CC4"/>
-    <mergeCell ref="CD4:CK4"/>
-    <mergeCell ref="CL4:CS4"/>
-    <mergeCell ref="CT4:DA4"/>
-    <mergeCell ref="DB4:DI4"/>
-    <mergeCell ref="DJ4:DQ4"/>
-    <mergeCell ref="DR4:DY4"/>
-    <mergeCell ref="DZ4:EG4"/>
-    <mergeCell ref="EH4:EO4"/>
-    <mergeCell ref="EP4:EW4"/>
-    <mergeCell ref="EX4:FE4"/>
-    <mergeCell ref="FF4:FM4"/>
-    <mergeCell ref="FN4:FU4"/>
-    <mergeCell ref="FV4:GC4"/>
-    <mergeCell ref="GD4:GK4"/>
-    <mergeCell ref="GL4:GS4"/>
-    <mergeCell ref="GT4:HA4"/>
-    <mergeCell ref="HB4:HI4"/>
-    <mergeCell ref="HJ4:HQ4"/>
-    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="HB2:HQ2"/>
+    <mergeCell ref="HR2:IG2"/>
+    <mergeCell ref="IH2:IW2"/>
+    <mergeCell ref="DZ2:EO2"/>
+    <mergeCell ref="EP2:FE2"/>
+    <mergeCell ref="FF2:FU2"/>
+    <mergeCell ref="FV2:GK2"/>
+    <mergeCell ref="GL2:HA2"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="BN2:CC2"/>
+    <mergeCell ref="CD2:CS2"/>
+    <mergeCell ref="CT2:DI2"/>
+    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="IH3:IW3"/>
+    <mergeCell ref="AH1:AW1"/>
+    <mergeCell ref="AX1:BM1"/>
+    <mergeCell ref="BN1:CC1"/>
+    <mergeCell ref="CD1:CS1"/>
+    <mergeCell ref="CT1:DI1"/>
+    <mergeCell ref="DJ1:DY1"/>
+    <mergeCell ref="DZ1:EO1"/>
+    <mergeCell ref="EP1:FE1"/>
+    <mergeCell ref="FF1:FU1"/>
+    <mergeCell ref="FV1:GK1"/>
+    <mergeCell ref="GL1:HA1"/>
+    <mergeCell ref="HB1:HQ1"/>
+    <mergeCell ref="HR1:IG1"/>
+    <mergeCell ref="IH1:IW1"/>
+    <mergeCell ref="AH2:AW2"/>
     <mergeCell ref="HZ4:IG4"/>
     <mergeCell ref="IH4:IO4"/>
     <mergeCell ref="IP4:IW4"/>
@@ -27178,35 +27302,41 @@
     <mergeCell ref="GL3:HA3"/>
     <mergeCell ref="HB3:HQ3"/>
     <mergeCell ref="HR3:IG3"/>
-    <mergeCell ref="IH3:IW3"/>
-    <mergeCell ref="AH1:AW1"/>
-    <mergeCell ref="AX1:BM1"/>
-    <mergeCell ref="BN1:CC1"/>
-    <mergeCell ref="CD1:CS1"/>
-    <mergeCell ref="CT1:DI1"/>
-    <mergeCell ref="DJ1:DY1"/>
-    <mergeCell ref="DZ1:EO1"/>
-    <mergeCell ref="EP1:FE1"/>
-    <mergeCell ref="FF1:FU1"/>
-    <mergeCell ref="FV1:GK1"/>
-    <mergeCell ref="GL1:HA1"/>
-    <mergeCell ref="HB1:HQ1"/>
-    <mergeCell ref="HR1:IG1"/>
-    <mergeCell ref="IH1:IW1"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="BN2:CC2"/>
-    <mergeCell ref="CD2:CS2"/>
-    <mergeCell ref="CT2:DI2"/>
-    <mergeCell ref="DJ2:DY2"/>
-    <mergeCell ref="HB2:HQ2"/>
-    <mergeCell ref="HR2:IG2"/>
-    <mergeCell ref="IH2:IW2"/>
-    <mergeCell ref="DZ2:EO2"/>
-    <mergeCell ref="EP2:FE2"/>
-    <mergeCell ref="FF2:FU2"/>
-    <mergeCell ref="FV2:GK2"/>
-    <mergeCell ref="GL2:HA2"/>
+    <mergeCell ref="GL4:GS4"/>
+    <mergeCell ref="GT4:HA4"/>
+    <mergeCell ref="HB4:HI4"/>
+    <mergeCell ref="HJ4:HQ4"/>
+    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="EX4:FE4"/>
+    <mergeCell ref="FF4:FM4"/>
+    <mergeCell ref="FN4:FU4"/>
+    <mergeCell ref="FV4:GC4"/>
+    <mergeCell ref="GD4:GK4"/>
+    <mergeCell ref="DJ4:DQ4"/>
+    <mergeCell ref="DR4:DY4"/>
+    <mergeCell ref="DZ4:EG4"/>
+    <mergeCell ref="EH4:EO4"/>
+    <mergeCell ref="EP4:EW4"/>
+    <mergeCell ref="BV4:CC4"/>
+    <mergeCell ref="CD4:CK4"/>
+    <mergeCell ref="CL4:CS4"/>
+    <mergeCell ref="CT4:DA4"/>
+    <mergeCell ref="DB4:DI4"/>
+    <mergeCell ref="AH4:AO4"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="BN4:BU4"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="R3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>